<commit_message>
Added unit tests in test_chequing_account.py
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_chequing_account.xlsx
+++ b/tests/A02_pixell_test_plan_chequing_account.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>#VALUE!</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Developer:</t>
+  </si>
+  <si>
+    <t>Komalpreet Kaur</t>
   </si>
   <si>
     <t>Class Name:</t>
@@ -90,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +104,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -151,7 +160,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -418,85 +434,85 @@
   <cellXfs count="30">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="14" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -863,7 +879,9 @@
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="D3" s="9"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -872,17 +890,17 @@
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
       <c r="B4" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="1"/>
       <c r="B5" s="13"/>
       <c r="C5" s="3"/>
@@ -891,127 +909,127 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1"/>
       <c r="B6" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="44.25" customFormat="1" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="46.5" customFormat="1" s="16">
       <c r="A7" s="17"/>
       <c r="B7" s="18">
         <v>1</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="16">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25" customFormat="1" s="16">
       <c r="A8" s="17"/>
       <c r="B8" s="21">
         <v>2</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="16">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25" customFormat="1" s="16">
       <c r="A9" s="17"/>
       <c r="B9" s="18">
         <v>3</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="23"/>
       <c r="G9" s="20"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="16">
       <c r="A10" s="17"/>
       <c r="B10" s="18">
         <v>4</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25" customFormat="1" s="16">
       <c r="A11" s="17"/>
       <c r="B11" s="21">
         <v>5</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25" customFormat="1" s="16">
       <c r="A12" s="17"/>
       <c r="B12" s="18">
         <v>6</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="31.149999999999995" customFormat="1" s="16">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="16">
       <c r="A13" s="17"/>
       <c r="B13" s="18">
         <v>7</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="23"/>
@@ -1023,10 +1041,10 @@
         <v>8</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="23"/>
@@ -1220,7 +1238,7 @@
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1"/>
       <c r="B32" s="25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>

</xml_diff>